<commit_message>
Fixed code related to driver close
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Web.xlsx
+++ b/src/test/resources/testData/Web.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19401"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsukdeo\OneDrive - Royal college of General Practitioners\My Documents\NetBeansProjects\nishaan_automation_framework\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DCBACD9-46F9-45F2-B8E3-04CCD3AFA22A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="MasterData" sheetId="9" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <sheet name="TermsAndConditionsInfoData" sheetId="7" r:id="rId7"/>
     <sheet name="PaymentInfoData" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="229">
   <si>
     <t>ValidationInfoData</t>
   </si>
@@ -527,13 +526,205 @@
   </si>
   <si>
     <t>IsCorrespondenceDifferent</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Brandon</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>Alexandra</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>Zak</t>
+  </si>
+  <si>
+    <t>Lara</t>
+  </si>
+  <si>
+    <t>Moran-Jarvis</t>
+  </si>
+  <si>
+    <t>Fry-Jarvis</t>
+  </si>
+  <si>
+    <t>Davies-Jarvis</t>
+  </si>
+  <si>
+    <t>Norton-Jarvis</t>
+  </si>
+  <si>
+    <t>Craig-Jarvis</t>
+  </si>
+  <si>
+    <t>Black-Jarvis</t>
+  </si>
+  <si>
+    <t>Crawford-Jarvis</t>
+  </si>
+  <si>
+    <t>Howarth-Jarvis</t>
+  </si>
+  <si>
+    <t>Cartwright-Jarvis</t>
+  </si>
+  <si>
+    <t>GabrielMoran@rhyta.com</t>
+  </si>
+  <si>
+    <t>BrandonFry@rhyta.com</t>
+  </si>
+  <si>
+    <t>MorganDavies@gustr.com</t>
+  </si>
+  <si>
+    <t>AlexandraNorton@cuvox.de</t>
+  </si>
+  <si>
+    <t>ChelseaCraig@fleckens.hu</t>
+  </si>
+  <si>
+    <t>GeorgiaBlack@cuvox.de</t>
+  </si>
+  <si>
+    <t>HarryCrawford@gustr.com</t>
+  </si>
+  <si>
+    <t>ZakHowarth@cuvox.de</t>
+  </si>
+  <si>
+    <t>LaraCartwright@armyspy.com</t>
+  </si>
+  <si>
+    <t>07080549365</t>
+  </si>
+  <si>
+    <t>07903046194</t>
+  </si>
+  <si>
+    <t>07932663801</t>
+  </si>
+  <si>
+    <t>07880953349</t>
+  </si>
+  <si>
+    <t>07952520657</t>
+  </si>
+  <si>
+    <t>07001350696</t>
+  </si>
+  <si>
+    <t>07980745917</t>
+  </si>
+  <si>
+    <t>07949185564</t>
+  </si>
+  <si>
+    <t>07817828398</t>
+  </si>
+  <si>
+    <t>45 Quay Street</t>
+  </si>
+  <si>
+    <t>58 Essex Rd</t>
+  </si>
+  <si>
+    <t>70 Davids Lane</t>
+  </si>
+  <si>
+    <t>68 Victoria Road</t>
+  </si>
+  <si>
+    <t>73 Roker Terrace</t>
+  </si>
+  <si>
+    <t>89 Haslemere Road</t>
+  </si>
+  <si>
+    <t>79 Ockham Road</t>
+  </si>
+  <si>
+    <t>59 Crown Street</t>
+  </si>
+  <si>
+    <t>58 Tonbridge Rd</t>
+  </si>
+  <si>
+    <t>NANT-Y-DUGOED</t>
+  </si>
+  <si>
+    <t>TATTINGSTONE</t>
+  </si>
+  <si>
+    <t>SUFFIELD</t>
+  </si>
+  <si>
+    <t>LITTLE BRAMPTON</t>
+  </si>
+  <si>
+    <t>LANGRISH</t>
+  </si>
+  <si>
+    <t>EASTON ON THE HILL</t>
+  </si>
+  <si>
+    <t>EAST VILLAGE</t>
+  </si>
+  <si>
+    <t>LONDON</t>
+  </si>
+  <si>
+    <t>COPTHORNE</t>
+  </si>
+  <si>
+    <t>SY21 1TW</t>
+  </si>
+  <si>
+    <t>IP9 1SR</t>
+  </si>
+  <si>
+    <t>YO13 1DF</t>
+  </si>
+  <si>
+    <t>SY7 0ND</t>
+  </si>
+  <si>
+    <t>GU32 8LF</t>
+  </si>
+  <si>
+    <t>PE9 3AE</t>
+  </si>
+  <si>
+    <t>EX17 0BH</t>
+  </si>
+  <si>
+    <t>SW1P 0PP</t>
+  </si>
+  <si>
+    <t>RH10 4GL</t>
+  </si>
+  <si>
+    <t>Portugal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,7 +764,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -675,51 +866,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -783,26 +929,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -819,13 +950,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -835,13 +964,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1157,14 +1286,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -1176,7 +1305,7 @@
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="33.85546875" bestFit="1" customWidth="1"/>
@@ -1205,61 +1334,61 @@
     <col min="37" max="37" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="19.5">
-      <c r="A1" s="19"/>
-      <c r="B1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="23" t="s">
+    <row r="1" spans="1:37" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="16"/>
+      <c r="B1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="23" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="26" t="s">
+      <c r="O1" s="23"/>
+      <c r="P1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="23" t="s">
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="23" t="s">
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="23" t="s">
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="25"/>
-    </row>
-    <row r="2" spans="1:37" s="7" customFormat="1">
-      <c r="A2" s="20" t="s">
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="23"/>
+    </row>
+    <row r="2" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -1371,8 +1500,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
-      <c r="A3" s="21">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
         <v>1</v>
       </c>
       <c r="B3" s="14">
@@ -1402,7 +1531,7 @@
       <c r="J3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="19">
         <v>18578</v>
       </c>
       <c r="L3" s="11" t="s">
@@ -1429,12 +1558,22 @@
       <c r="S3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="14">
+      <c r="T3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y3" s="20">
         <v>43465</v>
       </c>
       <c r="Z3" s="11" t="s">
@@ -1474,8 +1613,8 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
-      <c r="A4" s="21">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
         <v>2</v>
       </c>
       <c r="B4" s="14">
@@ -1505,7 +1644,7 @@
       <c r="J4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="19">
         <v>28459</v>
       </c>
       <c r="L4" s="11" t="s">
@@ -1537,7 +1676,7 @@
       <c r="V4" s="11"/>
       <c r="W4" s="11"/>
       <c r="X4" s="15"/>
-      <c r="Y4" s="14">
+      <c r="Y4" s="20">
         <v>43281</v>
       </c>
       <c r="Z4" s="11" t="s">
@@ -1577,8 +1716,8 @@
         <v>722</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
-      <c r="A5" s="21">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
         <v>3</v>
       </c>
       <c r="B5" s="14">
@@ -1608,7 +1747,7 @@
       <c r="J5" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="19">
         <v>33797</v>
       </c>
       <c r="L5" s="11" t="s">
@@ -1650,7 +1789,7 @@
       <c r="X5" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="14">
+      <c r="Y5" s="20">
         <v>43539</v>
       </c>
       <c r="Z5" s="11" t="s">
@@ -1690,8 +1829,8 @@
         <v>289</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
-      <c r="A6" s="21">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
         <v>4</v>
       </c>
       <c r="B6" s="14">
@@ -1721,7 +1860,7 @@
       <c r="J6" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="19">
         <v>20993</v>
       </c>
       <c r="L6" s="11" t="s">
@@ -1753,7 +1892,7 @@
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
       <c r="X6" s="15"/>
-      <c r="Y6" s="14">
+      <c r="Y6" s="20">
         <v>43322</v>
       </c>
       <c r="Z6" s="11" t="s">
@@ -1793,8 +1932,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
-      <c r="A7" s="21">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
         <v>5</v>
       </c>
       <c r="B7" s="14">
@@ -1824,7 +1963,7 @@
       <c r="J7" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="19">
         <v>21299</v>
       </c>
       <c r="L7" s="11" t="s">
@@ -1856,7 +1995,7 @@
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
       <c r="X7" s="15"/>
-      <c r="Y7" s="14">
+      <c r="Y7" s="20">
         <v>43483</v>
       </c>
       <c r="Z7" s="11" t="s">
@@ -1896,8 +2035,8 @@
         <v>520</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
-      <c r="A8" s="21">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
         <v>6</v>
       </c>
       <c r="B8" s="14">
@@ -1927,7 +2066,7 @@
       <c r="J8" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="19">
         <v>31114</v>
       </c>
       <c r="L8" s="11" t="s">
@@ -1959,7 +2098,7 @@
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
       <c r="X8" s="15"/>
-      <c r="Y8" s="14">
+      <c r="Y8" s="20">
         <v>44170</v>
       </c>
       <c r="Z8" s="11" t="s">
@@ -1999,8 +2138,8 @@
         <v>846</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
-      <c r="A9" s="21">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
         <v>7</v>
       </c>
       <c r="B9" s="14">
@@ -2030,7 +2169,7 @@
       <c r="J9" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="19">
         <v>22729</v>
       </c>
       <c r="L9" s="11" t="s">
@@ -2072,7 +2211,7 @@
       <c r="X9" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="Y9" s="14">
+      <c r="Y9" s="20">
         <v>44284</v>
       </c>
       <c r="Z9" s="11" t="s">
@@ -2112,8 +2251,8 @@
         <v>972</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
-      <c r="A10" s="21">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
         <v>8</v>
       </c>
       <c r="B10" s="14">
@@ -2143,7 +2282,7 @@
       <c r="J10" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="19">
         <v>27263</v>
       </c>
       <c r="L10" s="11" t="s">
@@ -2175,7 +2314,7 @@
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>
       <c r="X10" s="15"/>
-      <c r="Y10" s="14">
+      <c r="Y10" s="20">
         <v>44906</v>
       </c>
       <c r="Z10" s="11" t="s">
@@ -2215,8 +2354,8 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
-      <c r="A11" s="21">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
         <v>9</v>
       </c>
       <c r="B11" s="14">
@@ -2246,7 +2385,7 @@
       <c r="J11" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="19">
         <v>24828</v>
       </c>
       <c r="L11" s="11" t="s">
@@ -2278,7 +2417,7 @@
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
       <c r="X11" s="15"/>
-      <c r="Y11" s="14">
+      <c r="Y11" s="20">
         <v>43708</v>
       </c>
       <c r="Z11" s="11" t="s">
@@ -2318,8 +2457,8 @@
         <v>542</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
-      <c r="A12" s="21">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
         <v>10</v>
       </c>
       <c r="B12" s="14">
@@ -2349,7 +2488,7 @@
       <c r="J12" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="19">
         <v>32954</v>
       </c>
       <c r="L12" s="11" t="s">
@@ -2381,7 +2520,7 @@
       <c r="V12" s="11"/>
       <c r="W12" s="11"/>
       <c r="X12" s="15"/>
-      <c r="Y12" s="14">
+      <c r="Y12" s="20">
         <v>44255</v>
       </c>
       <c r="Z12" s="11" t="s">
@@ -2421,106 +2560,1033 @@
         <v>629</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15.75" thickBot="1">
-      <c r="A13" s="22">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
         <v>11</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="14">
         <v>350768</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="19">
         <v>26678</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="L13" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="M13" s="18" t="s">
+      <c r="M13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="N13" s="16" t="s">
+      <c r="N13" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="O13" s="18" t="s">
+      <c r="O13" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="P13" s="16" t="s">
+      <c r="P13" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="Q13" s="17" t="s">
+      <c r="Q13" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="R13" s="17" t="s">
+      <c r="R13" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="S13" s="17" t="s">
+      <c r="S13" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="T13" s="17"/>
-      <c r="U13" s="17"/>
-      <c r="V13" s="17"/>
-      <c r="W13" s="17"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="16">
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="20">
         <v>43539</v>
       </c>
-      <c r="Z13" s="17" t="s">
+      <c r="Z13" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="AA13" s="17">
+      <c r="AA13" s="11">
         <v>3456</v>
       </c>
-      <c r="AB13" s="17" t="s">
+      <c r="AB13" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AC13" s="17" t="s">
+      <c r="AC13" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AD13" s="18" t="s">
+      <c r="AD13" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="AE13" s="16" t="s">
+      <c r="AE13" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AF13" s="17" t="s">
+      <c r="AF13" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="AG13" s="18" t="s">
+      <c r="AG13" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="AH13" s="16" t="s">
+      <c r="AH13" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="AI13" s="17">
+      <c r="AI13" s="11">
         <v>1</v>
       </c>
-      <c r="AJ13" s="17">
+      <c r="AJ13" s="11">
         <v>2020</v>
       </c>
-      <c r="AK13" s="18">
+      <c r="AK13" s="15">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>12</v>
+      </c>
+      <c r="B14" s="14">
+        <v>350417</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="K14" s="19">
+        <v>23529</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q14" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="20">
+        <v>43708</v>
+      </c>
+      <c r="Z14" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA14" s="11">
+        <v>8765</v>
+      </c>
+      <c r="AB14" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC14" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD14" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE14" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG14" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH14" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI14" s="11">
+        <v>7</v>
+      </c>
+      <c r="AJ14" s="11">
+        <v>2023</v>
+      </c>
+      <c r="AK14" s="15">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>13</v>
+      </c>
+      <c r="B15" s="14">
+        <v>350419</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="K15" s="19">
+        <v>31384</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="20">
+        <v>43539</v>
+      </c>
+      <c r="Z15" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA15" s="11">
+        <v>7654</v>
+      </c>
+      <c r="AB15" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC15" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD15" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF15" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI15" s="11">
+        <v>6</v>
+      </c>
+      <c r="AJ15" s="11">
+        <v>2022</v>
+      </c>
+      <c r="AK15" s="15">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>14</v>
+      </c>
+      <c r="B16" s="14">
+        <v>350768</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="K16" s="19">
+        <v>24822</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="O16" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q16" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="20">
+        <v>43539</v>
+      </c>
+      <c r="Z16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA16" s="11">
+        <v>3456</v>
+      </c>
+      <c r="AB16" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC16" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD16" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE16" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF16" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG16" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH16" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI16" s="11">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="11">
+        <v>2020</v>
+      </c>
+      <c r="AK16" s="15">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>15</v>
+      </c>
+      <c r="B17" s="14">
+        <v>350417</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K17" s="19">
+        <v>17028</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="O17" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="P17" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="S17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="20">
+        <v>44255</v>
+      </c>
+      <c r="Z17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA17" s="11">
+        <v>8765</v>
+      </c>
+      <c r="AB17" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC17" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD17" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE17" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF17" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG17" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI17" s="11">
+        <v>7</v>
+      </c>
+      <c r="AJ17" s="11">
+        <v>2023</v>
+      </c>
+      <c r="AK17" s="15">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="14">
+        <v>350419</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="K18" s="19">
+        <v>21697</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="N18" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="O18" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="P18" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q18" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="R18" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="S18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="20">
+        <v>44906</v>
+      </c>
+      <c r="Z18" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA18" s="11">
+        <v>7654</v>
+      </c>
+      <c r="AB18" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC18" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE18" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF18" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG18" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH18" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI18" s="11">
+        <v>6</v>
+      </c>
+      <c r="AJ18" s="11">
+        <v>2022</v>
+      </c>
+      <c r="AK18" s="15">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A19" s="18">
+        <v>17</v>
+      </c>
+      <c r="B19" s="14">
+        <v>350768</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="K19" s="19">
+        <v>17328</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M19" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="O19" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="P19" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q19" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="R19" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="S19" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="20">
+        <v>43539</v>
+      </c>
+      <c r="Z19" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA19" s="11">
+        <v>3456</v>
+      </c>
+      <c r="AB19" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC19" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD19" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE19" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH19" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI19" s="11">
+        <v>1</v>
+      </c>
+      <c r="AJ19" s="11">
+        <v>2020</v>
+      </c>
+      <c r="AK19" s="15">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A20" s="18">
+        <v>18</v>
+      </c>
+      <c r="B20" s="14">
+        <v>350417</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="K20" s="19">
+        <v>28298</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="O20" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="P20" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="R20" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="S20" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="20">
+        <v>43708</v>
+      </c>
+      <c r="Z20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA20" s="11">
+        <v>8765</v>
+      </c>
+      <c r="AB20" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC20" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD20" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE20" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF20" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG20" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH20" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI20" s="11">
+        <v>7</v>
+      </c>
+      <c r="AJ20" s="11">
+        <v>2023</v>
+      </c>
+      <c r="AK20" s="15">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A21" s="18">
+        <v>19</v>
+      </c>
+      <c r="B21" s="14">
+        <v>350419</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="K21" s="19">
+        <v>28621</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="O21" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="P21" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q21" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="R21" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="S21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="20">
+        <v>43483</v>
+      </c>
+      <c r="Z21" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA21" s="11">
+        <v>7654</v>
+      </c>
+      <c r="AB21" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC21" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD21" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE21" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF21" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG21" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH21" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI21" s="11">
+        <v>6</v>
+      </c>
+      <c r="AJ21" s="11">
+        <v>2022</v>
+      </c>
+      <c r="AK21" s="15">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A22" s="18">
+        <v>20</v>
+      </c>
+      <c r="B22" s="14">
+        <v>350768</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="K22" s="19">
+        <v>22737</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="N22" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="O22" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="P22" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q22" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="R22" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="S22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="20">
+        <v>44170</v>
+      </c>
+      <c r="Z22" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA22" s="11">
+        <v>3456</v>
+      </c>
+      <c r="AB22" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC22" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD22" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE22" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG22" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH22" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI22" s="11">
+        <v>1</v>
+      </c>
+      <c r="AJ22" s="11">
+        <v>2020</v>
+      </c>
+      <c r="AK22" s="15">
         <v>289</v>
       </c>
     </row>
@@ -2535,10 +3601,10 @@
     <mergeCell ref="H1:M1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="N4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="N3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="N4" r:id="rId3"/>
+    <hyperlink ref="N3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -2549,14 +3615,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="C12" sqref="C12:G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
@@ -2566,7 +3632,7 @@
     <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -2586,7 +3652,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>MasterData!B3</f>
         <v>350271</v>
@@ -2612,7 +3678,7 @@
         <v>RCGP1234</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>MasterData!B4</f>
         <v>350281</v>
@@ -2638,7 +3704,7 @@
         <v>RCGP1234</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>MasterData!B5</f>
         <v>350284</v>
@@ -2664,7 +3730,7 @@
         <v>RCGP1234</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>MasterData!B6</f>
         <v>350289</v>
@@ -2690,7 +3756,7 @@
         <v>RCGP1234</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>MasterData!B7</f>
         <v>350294</v>
@@ -2716,7 +3782,7 @@
         <v>RCGP1234</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>MasterData!B8</f>
         <v>350297</v>
@@ -2742,7 +3808,7 @@
         <v>RCGP1234</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>MasterData!B9</f>
         <v>350412</v>
@@ -2768,7 +3834,7 @@
         <v>RCGP1234</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>MasterData!B10</f>
         <v>350416</v>
@@ -2794,7 +3860,7 @@
         <v>RCGP1234</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <f>MasterData!B11</f>
         <v>350417</v>
@@ -2820,7 +3886,7 @@
         <v>RCGP1234</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>MasterData!B12</f>
         <v>350419</v>
@@ -2846,7 +3912,7 @@
         <v>RCGP1234</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>MasterData!B13</f>
         <v>350768</v>
@@ -2869,6 +3935,240 @@
       </c>
       <c r="G13" t="str">
         <f>MasterData!G13</f>
+        <v>RCGP1234</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f>MasterData!B14</f>
+        <v>350417</v>
+      </c>
+      <c r="C14" s="4" t="str">
+        <f>MasterData!C14</f>
+        <v>Moran-Jarvis</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>MasterData!D14</f>
+        <v>GabrielMoran@rhyta.com</v>
+      </c>
+      <c r="E14" t="str">
+        <f>MasterData!E14</f>
+        <v>Gabriel</v>
+      </c>
+      <c r="F14" t="str">
+        <f>MasterData!F14</f>
+        <v>RCGP1234</v>
+      </c>
+      <c r="G14" t="str">
+        <f>MasterData!G14</f>
+        <v>RCGP1234</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f>MasterData!B15</f>
+        <v>350419</v>
+      </c>
+      <c r="C15" s="4" t="str">
+        <f>MasterData!C15</f>
+        <v>Fry-Jarvis</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f>MasterData!D15</f>
+        <v>BrandonFry@rhyta.com</v>
+      </c>
+      <c r="E15" t="str">
+        <f>MasterData!E15</f>
+        <v>Brandon</v>
+      </c>
+      <c r="F15" t="str">
+        <f>MasterData!F15</f>
+        <v>RCGP1234</v>
+      </c>
+      <c r="G15" t="str">
+        <f>MasterData!G15</f>
+        <v>RCGP1234</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>MasterData!B16</f>
+        <v>350768</v>
+      </c>
+      <c r="C16" s="4" t="str">
+        <f>MasterData!C16</f>
+        <v>Davies-Jarvis</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f>MasterData!D16</f>
+        <v>MorganDavies@gustr.com</v>
+      </c>
+      <c r="E16" t="str">
+        <f>MasterData!E16</f>
+        <v>Morgan</v>
+      </c>
+      <c r="F16" t="str">
+        <f>MasterData!F16</f>
+        <v>RCGP1234</v>
+      </c>
+      <c r="G16" t="str">
+        <f>MasterData!G16</f>
+        <v>RCGP1234</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>MasterData!B17</f>
+        <v>350417</v>
+      </c>
+      <c r="C17" s="4" t="str">
+        <f>MasterData!C17</f>
+        <v>Norton-Jarvis</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>MasterData!D17</f>
+        <v>AlexandraNorton@cuvox.de</v>
+      </c>
+      <c r="E17" t="str">
+        <f>MasterData!E17</f>
+        <v>Alexandra</v>
+      </c>
+      <c r="F17" t="str">
+        <f>MasterData!F17</f>
+        <v>RCGP1234</v>
+      </c>
+      <c r="G17" t="str">
+        <f>MasterData!G17</f>
+        <v>RCGP1234</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>MasterData!B18</f>
+        <v>350419</v>
+      </c>
+      <c r="C18" s="4" t="str">
+        <f>MasterData!C18</f>
+        <v>Craig-Jarvis</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f>MasterData!D18</f>
+        <v>ChelseaCraig@fleckens.hu</v>
+      </c>
+      <c r="E18" t="str">
+        <f>MasterData!E18</f>
+        <v>Chelsea</v>
+      </c>
+      <c r="F18" t="str">
+        <f>MasterData!F18</f>
+        <v>RCGP1234</v>
+      </c>
+      <c r="G18" t="str">
+        <f>MasterData!G18</f>
+        <v>RCGP1234</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f>MasterData!B19</f>
+        <v>350768</v>
+      </c>
+      <c r="C19" s="4" t="str">
+        <f>MasterData!C19</f>
+        <v>Black-Jarvis</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f>MasterData!D19</f>
+        <v>GeorgiaBlack@cuvox.de</v>
+      </c>
+      <c r="E19" t="str">
+        <f>MasterData!E19</f>
+        <v>Georgia</v>
+      </c>
+      <c r="F19" t="str">
+        <f>MasterData!F19</f>
+        <v>RCGP1234</v>
+      </c>
+      <c r="G19" t="str">
+        <f>MasterData!G19</f>
+        <v>RCGP1234</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>MasterData!B20</f>
+        <v>350417</v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <f>MasterData!C20</f>
+        <v>Crawford-Jarvis</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>MasterData!D20</f>
+        <v>HarryCrawford@gustr.com</v>
+      </c>
+      <c r="E20" t="str">
+        <f>MasterData!E20</f>
+        <v>Harry</v>
+      </c>
+      <c r="F20" t="str">
+        <f>MasterData!F20</f>
+        <v>RCGP1234</v>
+      </c>
+      <c r="G20" t="str">
+        <f>MasterData!G20</f>
+        <v>RCGP1234</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f>MasterData!B21</f>
+        <v>350419</v>
+      </c>
+      <c r="C21" s="4" t="str">
+        <f>MasterData!C21</f>
+        <v>Howarth-Jarvis</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f>MasterData!D21</f>
+        <v>ZakHowarth@cuvox.de</v>
+      </c>
+      <c r="E21" t="str">
+        <f>MasterData!E21</f>
+        <v>Zak</v>
+      </c>
+      <c r="F21" t="str">
+        <f>MasterData!F21</f>
+        <v>RCGP1234</v>
+      </c>
+      <c r="G21" t="str">
+        <f>MasterData!G21</f>
+        <v>RCGP1234</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f>MasterData!B22</f>
+        <v>350768</v>
+      </c>
+      <c r="C22" s="4" t="str">
+        <f>MasterData!C22</f>
+        <v>Cartwright-Jarvis</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f>MasterData!D22</f>
+        <v>LaraCartwright@armyspy.com</v>
+      </c>
+      <c r="E22" t="str">
+        <f>MasterData!E22</f>
+        <v>Lara</v>
+      </c>
+      <c r="F22" t="str">
+        <f>MasterData!F22</f>
+        <v>RCGP1234</v>
+      </c>
+      <c r="G22" t="str">
+        <f>MasterData!G22</f>
         <v>RCGP1234</v>
       </c>
     </row>
@@ -2878,14 +4178,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
@@ -2895,7 +4195,7 @@
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="4" customFormat="1">
+    <row r="2" spans="2:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
@@ -2915,7 +4215,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="str">
         <f>MasterData!H3</f>
         <v>Mrs</v>
@@ -2941,7 +4241,7 @@
         <v>female</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="str">
         <f>MasterData!H4</f>
         <v>Mr</v>
@@ -2967,7 +4267,7 @@
         <v>male</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="str">
         <f>MasterData!H5</f>
         <v>Mr</v>
@@ -2993,7 +4293,7 @@
         <v>male</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="str">
         <f>MasterData!H6</f>
         <v>Mr</v>
@@ -3019,7 +4319,7 @@
         <v>male</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="str">
         <f>MasterData!H7</f>
         <v>Mr</v>
@@ -3045,7 +4345,7 @@
         <v>male</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="str">
         <f>MasterData!H8</f>
         <v>Mrs</v>
@@ -3071,7 +4371,7 @@
         <v>female</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="str">
         <f>MasterData!H9</f>
         <v>Ms</v>
@@ -3097,7 +4397,7 @@
         <v>female</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="str">
         <f>MasterData!H10</f>
         <v>Mr</v>
@@ -3123,7 +4423,7 @@
         <v>male</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="str">
         <f>MasterData!H11</f>
         <v>Ms</v>
@@ -3149,7 +4449,7 @@
         <v>female</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="str">
         <f>MasterData!H12</f>
         <v>Ms</v>
@@ -3175,7 +4475,7 @@
         <v>female</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="str">
         <f>MasterData!H13</f>
         <v>Ms</v>
@@ -3198,6 +4498,240 @@
       </c>
       <c r="G13" s="1" t="str">
         <f>MasterData!M13</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="str">
+        <f>MasterData!H14</f>
+        <v>Mr</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>MasterData!I14</f>
+        <v>Gabriel</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>MasterData!J14</f>
+        <v>Moran-Jarvis</v>
+      </c>
+      <c r="E14" s="2">
+        <f>MasterData!K14</f>
+        <v>23529</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f>MasterData!L14</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <f>MasterData!M14</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="str">
+        <f>MasterData!H15</f>
+        <v>Mr</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f>MasterData!I15</f>
+        <v>Brandon</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f>MasterData!J15</f>
+        <v>Fry-Jarvis</v>
+      </c>
+      <c r="E15" s="2">
+        <f>MasterData!K15</f>
+        <v>31384</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <f>MasterData!L15</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <f>MasterData!M15</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="str">
+        <f>MasterData!H16</f>
+        <v>Mrs</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>MasterData!I16</f>
+        <v>Morgan</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f>MasterData!J16</f>
+        <v>Davies-Jarvis</v>
+      </c>
+      <c r="E16" s="2">
+        <f>MasterData!K16</f>
+        <v>24822</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <f>MasterData!L16</f>
+        <v>Ukraine</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <f>MasterData!M16</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="str">
+        <f>MasterData!H17</f>
+        <v>Mrs</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f>MasterData!I17</f>
+        <v>Alexandra</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>MasterData!J17</f>
+        <v>Norton-Jarvis</v>
+      </c>
+      <c r="E17" s="2">
+        <f>MasterData!K17</f>
+        <v>17028</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <f>MasterData!L17</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <f>MasterData!M17</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="str">
+        <f>MasterData!H18</f>
+        <v>Ms</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f>MasterData!I18</f>
+        <v>Chelsea</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f>MasterData!J18</f>
+        <v>Craig-Jarvis</v>
+      </c>
+      <c r="E18" s="2">
+        <f>MasterData!K18</f>
+        <v>21697</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f>MasterData!L18</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f>MasterData!M18</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="str">
+        <f>MasterData!H19</f>
+        <v>Ms</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f>MasterData!I19</f>
+        <v>Georgia</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f>MasterData!J19</f>
+        <v>Black-Jarvis</v>
+      </c>
+      <c r="E19" s="2">
+        <f>MasterData!K19</f>
+        <v>17328</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <f>MasterData!L19</f>
+        <v>Ukraine</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <f>MasterData!M19</f>
+        <v>female</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="str">
+        <f>MasterData!H20</f>
+        <v>Mr</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f>MasterData!I20</f>
+        <v>Harry</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>MasterData!J20</f>
+        <v>Crawford-Jarvis</v>
+      </c>
+      <c r="E20" s="2">
+        <f>MasterData!K20</f>
+        <v>28298</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <f>MasterData!L20</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <f>MasterData!M20</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="str">
+        <f>MasterData!H21</f>
+        <v>Mr</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f>MasterData!I21</f>
+        <v>Zak</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f>MasterData!J21</f>
+        <v>Howarth-Jarvis</v>
+      </c>
+      <c r="E21" s="2">
+        <f>MasterData!K21</f>
+        <v>28621</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <f>MasterData!L21</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="G21" s="1" t="str">
+        <f>MasterData!M21</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="str">
+        <f>MasterData!H22</f>
+        <v>Mrs</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f>MasterData!I22</f>
+        <v>Lara</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f>MasterData!J22</f>
+        <v>Cartwright-Jarvis</v>
+      </c>
+      <c r="E22" s="2">
+        <f>MasterData!K22</f>
+        <v>22737</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <f>MasterData!L22</f>
+        <v>Ukraine</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <f>MasterData!M22</f>
         <v>female</v>
       </c>
     </row>
@@ -3207,20 +4741,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -3228,7 +4762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="str">
         <f>MasterData!N3</f>
         <v>AliciaIngram@rhyta.com</v>
@@ -3238,7 +4772,7 @@
         <v>07839760235</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>MasterData!N4</f>
         <v>LouisIqbal@superrito.com</v>
@@ -3248,7 +4782,7 @@
         <v>07864131744</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
         <f>MasterData!N5</f>
         <v>LukeThompson@jourrapide.com</v>
@@ -3258,7 +4792,7 @@
         <v>07718131703</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
         <f>MasterData!N6</f>
         <v>FinlayMoore@jourrapide.com</v>
@@ -3268,7 +4802,7 @@
         <v>07041735026</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f>MasterData!N7</f>
         <v>LukeGill@superrito.com</v>
@@ -3278,7 +4812,7 @@
         <v>07030632233</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f>MasterData!N8</f>
         <v>MadeleineMetcalfe@armyspy.com</v>
@@ -3288,7 +4822,7 @@
         <v>07957875775</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f>MasterData!N9</f>
         <v>MelissaBrowne@einrot.com</v>
@@ -3298,7 +4832,7 @@
         <v>07978149613</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
         <f>MasterData!N10</f>
         <v>AlfieThompson@armyspy.com</v>
@@ -3308,7 +4842,7 @@
         <v>07909967393</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>MasterData!N11</f>
         <v>ScarlettHargreaves@jourrapide.com</v>
@@ -3318,7 +4852,7 @@
         <v>07825307858</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>MasterData!N12</f>
         <v>NiamhJarvis@rhyta.com</v>
@@ -3328,7 +4862,7 @@
         <v>07719820316</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>MasterData!N13</f>
         <v>SofiaMistry@armyspy.com</v>
@@ -3336,6 +4870,96 @@
       <c r="C13" s="5" t="str">
         <f>MasterData!O13</f>
         <v>07801131508</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f>MasterData!N14</f>
+        <v>GabrielMoran@rhyta.com</v>
+      </c>
+      <c r="C14" s="5" t="str">
+        <f>MasterData!O14</f>
+        <v>07080549365</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <f>MasterData!N15</f>
+        <v>BrandonFry@rhyta.com</v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <f>MasterData!O15</f>
+        <v>07903046194</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="str">
+        <f>MasterData!N16</f>
+        <v>MorganDavies@gustr.com</v>
+      </c>
+      <c r="C16" s="5" t="str">
+        <f>MasterData!O16</f>
+        <v>07932663801</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <f>MasterData!N17</f>
+        <v>AlexandraNorton@cuvox.de</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <f>MasterData!O17</f>
+        <v>07880953349</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="str">
+        <f>MasterData!N18</f>
+        <v>ChelseaCraig@fleckens.hu</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f>MasterData!O18</f>
+        <v>07952520657</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="str">
+        <f>MasterData!N19</f>
+        <v>GeorgiaBlack@cuvox.de</v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <f>MasterData!O19</f>
+        <v>07001350696</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="str">
+        <f>MasterData!N20</f>
+        <v>HarryCrawford@gustr.com</v>
+      </c>
+      <c r="C20" s="5" t="str">
+        <f>MasterData!O20</f>
+        <v>07980745917</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <f>MasterData!N21</f>
+        <v>ZakHowarth@cuvox.de</v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <f>MasterData!O21</f>
+        <v>07949185564</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
+        <f>MasterData!N22</f>
+        <v>LaraCartwright@armyspy.com</v>
+      </c>
+      <c r="C22" s="5" t="str">
+        <f>MasterData!O22</f>
+        <v>07817828398</v>
       </c>
     </row>
   </sheetData>
@@ -3344,14 +4968,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B2:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J23"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showZeros="0" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
@@ -3364,7 +4988,7 @@
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
@@ -3393,7 +5017,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="str">
         <f>MasterData!P3</f>
         <v>70 Holburn Lane</v>
@@ -3410,28 +5034,28 @@
         <f>MasterData!S3</f>
         <v>United Kingdom</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="5" t="str">
         <f>MasterData!T3</f>
-        <v>0</v>
-      </c>
-      <c r="G3">
+        <v>Yes</v>
+      </c>
+      <c r="G3" t="str">
         <f>MasterData!U3</f>
-        <v>0</v>
-      </c>
-      <c r="H3">
+        <v>123 Fake street</v>
+      </c>
+      <c r="H3" t="str">
         <f>MasterData!V3</f>
-        <v>0</v>
-      </c>
-      <c r="I3">
+        <v>Makebelieve land</v>
+      </c>
+      <c r="I3" t="str">
         <f>MasterData!W3</f>
-        <v>0</v>
-      </c>
-      <c r="J3">
+        <v>FA12KE</v>
+      </c>
+      <c r="J3" t="str">
         <f>MasterData!X3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10">
+        <v>Portugal</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>MasterData!P4</f>
         <v>19 Hertingfordbury Rd</v>
@@ -3469,7 +5093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
         <f>MasterData!P5</f>
         <v>89 Glandovey Terrace</v>
@@ -3507,7 +5131,7 @@
         <v>Spain</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
         <f>MasterData!P6</f>
         <v>90 Baldock Street</v>
@@ -3545,7 +5169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f>MasterData!P7</f>
         <v>91 Scotsburn Rd</v>
@@ -3583,7 +5207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f>MasterData!P8</f>
         <v>97 Berkeley Rd</v>
@@ -3621,7 +5245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f>MasterData!P9</f>
         <v>60 Prince Consort Road</v>
@@ -3659,7 +5283,7 @@
         <v>France</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
         <f>MasterData!P10</f>
         <v>25 Great North Road</v>
@@ -3697,7 +5321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>MasterData!P11</f>
         <v>56 Thirsk Road</v>
@@ -3735,7 +5359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>MasterData!P12</f>
         <v>7 Old Edinburgh Road</v>
@@ -3773,7 +5397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>MasterData!P13</f>
         <v>94 Maidstone Road</v>
@@ -3808,6 +5432,386 @@
       </c>
       <c r="J13">
         <f>MasterData!X13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f>MasterData!P14</f>
+        <v>45 Quay Street</v>
+      </c>
+      <c r="C14" t="str">
+        <f>MasterData!Q14</f>
+        <v>NANT-Y-DUGOED</v>
+      </c>
+      <c r="D14" t="str">
+        <f>MasterData!R14</f>
+        <v>SY21 1TW</v>
+      </c>
+      <c r="E14" t="str">
+        <f>MasterData!S14</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="F14" s="5">
+        <f>MasterData!T14</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f>MasterData!U14</f>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f>MasterData!V14</f>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f>MasterData!W14</f>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f>MasterData!X14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <f>MasterData!P15</f>
+        <v>58 Essex Rd</v>
+      </c>
+      <c r="C15" t="str">
+        <f>MasterData!Q15</f>
+        <v>TATTINGSTONE</v>
+      </c>
+      <c r="D15" t="str">
+        <f>MasterData!R15</f>
+        <v>IP9 1SR</v>
+      </c>
+      <c r="E15" t="str">
+        <f>MasterData!S15</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="F15" s="5">
+        <f>MasterData!T15</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f>MasterData!U15</f>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f>MasterData!V15</f>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f>MasterData!W15</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f>MasterData!X15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="str">
+        <f>MasterData!P16</f>
+        <v>70 Davids Lane</v>
+      </c>
+      <c r="C16" t="str">
+        <f>MasterData!Q16</f>
+        <v>SUFFIELD</v>
+      </c>
+      <c r="D16" t="str">
+        <f>MasterData!R16</f>
+        <v>YO13 1DF</v>
+      </c>
+      <c r="E16" t="str">
+        <f>MasterData!S16</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="F16" s="5">
+        <f>MasterData!T16</f>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f>MasterData!U16</f>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f>MasterData!V16</f>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f>MasterData!W16</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f>MasterData!X16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <f>MasterData!P17</f>
+        <v>68 Victoria Road</v>
+      </c>
+      <c r="C17" t="str">
+        <f>MasterData!Q17</f>
+        <v>LITTLE BRAMPTON</v>
+      </c>
+      <c r="D17" t="str">
+        <f>MasterData!R17</f>
+        <v>SY7 0ND</v>
+      </c>
+      <c r="E17" t="str">
+        <f>MasterData!S17</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="F17" s="5">
+        <f>MasterData!T17</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f>MasterData!U17</f>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f>MasterData!V17</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f>MasterData!W17</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>MasterData!X17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" t="str">
+        <f>MasterData!P18</f>
+        <v>73 Roker Terrace</v>
+      </c>
+      <c r="C18" t="str">
+        <f>MasterData!Q18</f>
+        <v>LANGRISH</v>
+      </c>
+      <c r="D18" t="str">
+        <f>MasterData!R18</f>
+        <v>GU32 8LF</v>
+      </c>
+      <c r="E18" t="str">
+        <f>MasterData!S18</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="F18" s="5">
+        <f>MasterData!T18</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f>MasterData!U18</f>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f>MasterData!V18</f>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f>MasterData!W18</f>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f>MasterData!X18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="str">
+        <f>MasterData!P19</f>
+        <v>89 Haslemere Road</v>
+      </c>
+      <c r="C19" t="str">
+        <f>MasterData!Q19</f>
+        <v>EASTON ON THE HILL</v>
+      </c>
+      <c r="D19" t="str">
+        <f>MasterData!R19</f>
+        <v>PE9 3AE</v>
+      </c>
+      <c r="E19" t="str">
+        <f>MasterData!S19</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="F19" s="5">
+        <f>MasterData!T19</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>MasterData!U19</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f>MasterData!V19</f>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f>MasterData!W19</f>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>MasterData!X19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="str">
+        <f>MasterData!P20</f>
+        <v>79 Ockham Road</v>
+      </c>
+      <c r="C20" t="str">
+        <f>MasterData!Q20</f>
+        <v>EAST VILLAGE</v>
+      </c>
+      <c r="D20" t="str">
+        <f>MasterData!R20</f>
+        <v>EX17 0BH</v>
+      </c>
+      <c r="E20" t="str">
+        <f>MasterData!S20</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="F20" s="5">
+        <f>MasterData!T20</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f>MasterData!U20</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f>MasterData!V20</f>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f>MasterData!W20</f>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f>MasterData!X20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <f>MasterData!P21</f>
+        <v>59 Crown Street</v>
+      </c>
+      <c r="C21" t="str">
+        <f>MasterData!Q21</f>
+        <v>LONDON</v>
+      </c>
+      <c r="D21" t="str">
+        <f>MasterData!R21</f>
+        <v>SW1P 0PP</v>
+      </c>
+      <c r="E21" t="str">
+        <f>MasterData!S21</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="F21" s="5">
+        <f>MasterData!T21</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>MasterData!U21</f>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f>MasterData!V21</f>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f>MasterData!W21</f>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f>MasterData!X21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
+        <f>MasterData!P22</f>
+        <v>58 Tonbridge Rd</v>
+      </c>
+      <c r="C22" t="str">
+        <f>MasterData!Q22</f>
+        <v>COPTHORNE</v>
+      </c>
+      <c r="D22" t="str">
+        <f>MasterData!R22</f>
+        <v>RH10 4GL</v>
+      </c>
+      <c r="E22" t="str">
+        <f>MasterData!S22</f>
+        <v>United Kingdom</v>
+      </c>
+      <c r="F22" s="5">
+        <f>MasterData!T22</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>MasterData!U22</f>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f>MasterData!V22</f>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f>MasterData!W22</f>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f>MasterData!X22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f>MasterData!P23</f>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f>MasterData!Q23</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>MasterData!R23</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f>MasterData!S23</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <f>MasterData!T23</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f>MasterData!U23</f>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f>MasterData!V23</f>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f>MasterData!W23</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f>MasterData!X23</f>
         <v>0</v>
       </c>
     </row>
@@ -3817,14 +5821,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B2:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
-      <selection activeCell="B12" sqref="B12:G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3834,7 +5838,7 @@
     <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="3" customFormat="1">
+    <row r="2" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>29</v>
       </c>
@@ -3854,7 +5858,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <f>MasterData!Y3</f>
         <v>43465</v>
@@ -3880,7 +5884,7 @@
         <v>Full Time: Three Year Scheme</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <f>MasterData!Y4</f>
         <v>43281</v>
@@ -3906,7 +5910,7 @@
         <v>Full Time: Four Year Scheme</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <f>MasterData!Y5</f>
         <v>43539</v>
@@ -3932,7 +5936,7 @@
         <v>Less Than Full Time: 76% or More</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <f>MasterData!Y6</f>
         <v>43322</v>
@@ -3958,7 +5962,7 @@
         <v>Less Than Full Time: 75% or Less</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <f>MasterData!Y7</f>
         <v>43483</v>
@@ -3984,7 +5988,7 @@
         <v>Less Than Full Time: 76% or More</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <f>MasterData!Y8</f>
         <v>44170</v>
@@ -4010,7 +6014,7 @@
         <v>Full Time: Three Year Scheme</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <f>MasterData!Y9</f>
         <v>44284</v>
@@ -4036,7 +6040,7 @@
         <v>Full Time: Four Year Scheme</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f>MasterData!Y10</f>
         <v>44906</v>
@@ -4062,7 +6066,7 @@
         <v>Less Than Full Time: 76% or More</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>MasterData!Y11</f>
         <v>43708</v>
@@ -4088,7 +6092,7 @@
         <v>Less Than Full Time: 75% or Less</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f>MasterData!Y12</f>
         <v>44255</v>
@@ -4114,7 +6118,7 @@
         <v>Less Than Full Time: 76% or More</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f>MasterData!Y13</f>
         <v>43539</v>
@@ -4137,6 +6141,240 @@
       </c>
       <c r="G13" t="str">
         <f>MasterData!AD13</f>
+        <v>Less Than Full Time: 76% or More</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <f>MasterData!Y14</f>
+        <v>43708</v>
+      </c>
+      <c r="C14" t="str">
+        <f>MasterData!Z14</f>
+        <v>No</v>
+      </c>
+      <c r="D14">
+        <f>MasterData!AA14</f>
+        <v>8765</v>
+      </c>
+      <c r="E14" t="str">
+        <f>MasterData!AB14</f>
+        <v>Wales</v>
+      </c>
+      <c r="F14" t="str">
+        <f>MasterData!AC14</f>
+        <v>UK - Wales (inc Cardiff &amp; Swansea)</v>
+      </c>
+      <c r="G14" t="str">
+        <f>MasterData!AD14</f>
+        <v>Less Than Full Time: 75% or Less</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <f>MasterData!Y15</f>
+        <v>43539</v>
+      </c>
+      <c r="C15" t="str">
+        <f>MasterData!Z15</f>
+        <v>Yes</v>
+      </c>
+      <c r="D15">
+        <f>MasterData!AA15</f>
+        <v>7654</v>
+      </c>
+      <c r="E15" t="str">
+        <f>MasterData!AB15</f>
+        <v>Wessex</v>
+      </c>
+      <c r="F15" t="str">
+        <f>MasterData!AC15</f>
+        <v>UK - Dundee</v>
+      </c>
+      <c r="G15" t="str">
+        <f>MasterData!AD15</f>
+        <v>Less Than Full Time: 76% or More</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <f>MasterData!Y16</f>
+        <v>43539</v>
+      </c>
+      <c r="C16" t="str">
+        <f>MasterData!Z16</f>
+        <v>Yes</v>
+      </c>
+      <c r="D16">
+        <f>MasterData!AA16</f>
+        <v>3456</v>
+      </c>
+      <c r="E16" t="str">
+        <f>MasterData!AB16</f>
+        <v>Oxford</v>
+      </c>
+      <c r="F16" t="str">
+        <f>MasterData!AC16</f>
+        <v>OC - Zimbabwe</v>
+      </c>
+      <c r="G16" t="str">
+        <f>MasterData!AD16</f>
+        <v>Less Than Full Time: 76% or More</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <f>MasterData!Y17</f>
+        <v>44255</v>
+      </c>
+      <c r="C17" t="str">
+        <f>MasterData!Z17</f>
+        <v>No</v>
+      </c>
+      <c r="D17">
+        <f>MasterData!AA17</f>
+        <v>8765</v>
+      </c>
+      <c r="E17" t="str">
+        <f>MasterData!AB17</f>
+        <v>Wales</v>
+      </c>
+      <c r="F17" t="str">
+        <f>MasterData!AC17</f>
+        <v>UK - Wales (inc Cardiff &amp; Swansea)</v>
+      </c>
+      <c r="G17" t="str">
+        <f>MasterData!AD17</f>
+        <v>Less Than Full Time: 75% or Less</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <f>MasterData!Y18</f>
+        <v>44906</v>
+      </c>
+      <c r="C18" t="str">
+        <f>MasterData!Z18</f>
+        <v>Yes</v>
+      </c>
+      <c r="D18">
+        <f>MasterData!AA18</f>
+        <v>7654</v>
+      </c>
+      <c r="E18" t="str">
+        <f>MasterData!AB18</f>
+        <v>Wessex</v>
+      </c>
+      <c r="F18" t="str">
+        <f>MasterData!AC18</f>
+        <v>UK - Dundee</v>
+      </c>
+      <c r="G18" t="str">
+        <f>MasterData!AD18</f>
+        <v>Less Than Full Time: 76% or More</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <f>MasterData!Y19</f>
+        <v>43539</v>
+      </c>
+      <c r="C19" t="str">
+        <f>MasterData!Z19</f>
+        <v>Yes</v>
+      </c>
+      <c r="D19">
+        <f>MasterData!AA19</f>
+        <v>3456</v>
+      </c>
+      <c r="E19" t="str">
+        <f>MasterData!AB19</f>
+        <v>Oxford</v>
+      </c>
+      <c r="F19" t="str">
+        <f>MasterData!AC19</f>
+        <v>OC - Zimbabwe</v>
+      </c>
+      <c r="G19" t="str">
+        <f>MasterData!AD19</f>
+        <v>Less Than Full Time: 76% or More</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <f>MasterData!Y20</f>
+        <v>43708</v>
+      </c>
+      <c r="C20" t="str">
+        <f>MasterData!Z20</f>
+        <v>No</v>
+      </c>
+      <c r="D20">
+        <f>MasterData!AA20</f>
+        <v>8765</v>
+      </c>
+      <c r="E20" t="str">
+        <f>MasterData!AB20</f>
+        <v>Wales</v>
+      </c>
+      <c r="F20" t="str">
+        <f>MasterData!AC20</f>
+        <v>UK - Wales (inc Cardiff &amp; Swansea)</v>
+      </c>
+      <c r="G20" t="str">
+        <f>MasterData!AD20</f>
+        <v>Less Than Full Time: 75% or Less</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <f>MasterData!Y21</f>
+        <v>43483</v>
+      </c>
+      <c r="C21" t="str">
+        <f>MasterData!Z21</f>
+        <v>Yes</v>
+      </c>
+      <c r="D21">
+        <f>MasterData!AA21</f>
+        <v>7654</v>
+      </c>
+      <c r="E21" t="str">
+        <f>MasterData!AB21</f>
+        <v>Wessex</v>
+      </c>
+      <c r="F21" t="str">
+        <f>MasterData!AC21</f>
+        <v>UK - Dundee</v>
+      </c>
+      <c r="G21" t="str">
+        <f>MasterData!AD21</f>
+        <v>Less Than Full Time: 76% or More</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <f>MasterData!Y22</f>
+        <v>44170</v>
+      </c>
+      <c r="C22" t="str">
+        <f>MasterData!Z22</f>
+        <v>Yes</v>
+      </c>
+      <c r="D22">
+        <f>MasterData!AA22</f>
+        <v>3456</v>
+      </c>
+      <c r="E22" t="str">
+        <f>MasterData!AB22</f>
+        <v>Oxford</v>
+      </c>
+      <c r="F22" t="str">
+        <f>MasterData!AC22</f>
+        <v>OC - Zimbabwe</v>
+      </c>
+      <c r="G22" t="str">
+        <f>MasterData!AD22</f>
         <v>Less Than Full Time: 76% or More</v>
       </c>
     </row>
@@ -4146,21 +6384,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B2:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
-      <selection activeCell="B12" sqref="B12:D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>35</v>
       </c>
@@ -4171,7 +6409,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="str">
         <f>MasterData!AE3</f>
         <v xml:space="preserve">No </v>
@@ -4185,7 +6423,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>MasterData!AE4</f>
         <v>Yes</v>
@@ -4199,7 +6437,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
         <f>MasterData!AE5</f>
         <v xml:space="preserve">No </v>
@@ -4213,7 +6451,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
         <f>MasterData!AE6</f>
         <v xml:space="preserve">No </v>
@@ -4227,7 +6465,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f>MasterData!AE7</f>
         <v>Yes</v>
@@ -4241,7 +6479,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f>MasterData!AE8</f>
         <v xml:space="preserve">No </v>
@@ -4255,7 +6493,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f>MasterData!AE9</f>
         <v>Yes</v>
@@ -4269,7 +6507,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
         <f>MasterData!AE10</f>
         <v xml:space="preserve">No </v>
@@ -4283,7 +6521,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>MasterData!AE11</f>
         <v xml:space="preserve">No </v>
@@ -4297,7 +6535,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>MasterData!AE12</f>
         <v>Yes</v>
@@ -4311,7 +6549,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>MasterData!AE13</f>
         <v xml:space="preserve">No </v>
@@ -4322,6 +6560,132 @@
       </c>
       <c r="D13" t="str">
         <f>MasterData!AG13</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f>MasterData!AE14</f>
+        <v xml:space="preserve">No </v>
+      </c>
+      <c r="C14" t="str">
+        <f>MasterData!AF14</f>
+        <v>Yes</v>
+      </c>
+      <c r="D14" t="str">
+        <f>MasterData!AG14</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <f>MasterData!AE15</f>
+        <v>Yes</v>
+      </c>
+      <c r="C15" t="str">
+        <f>MasterData!AF15</f>
+        <v>Yes</v>
+      </c>
+      <c r="D15" t="str">
+        <f>MasterData!AG15</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="str">
+        <f>MasterData!AE16</f>
+        <v xml:space="preserve">No </v>
+      </c>
+      <c r="C16" t="str">
+        <f>MasterData!AF16</f>
+        <v>No</v>
+      </c>
+      <c r="D16" t="str">
+        <f>MasterData!AG16</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <f>MasterData!AE17</f>
+        <v xml:space="preserve">No </v>
+      </c>
+      <c r="C17" t="str">
+        <f>MasterData!AF17</f>
+        <v>Yes</v>
+      </c>
+      <c r="D17" t="str">
+        <f>MasterData!AG17</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="str">
+        <f>MasterData!AE18</f>
+        <v>Yes</v>
+      </c>
+      <c r="C18" t="str">
+        <f>MasterData!AF18</f>
+        <v>Yes</v>
+      </c>
+      <c r="D18" t="str">
+        <f>MasterData!AG18</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="str">
+        <f>MasterData!AE19</f>
+        <v xml:space="preserve">No </v>
+      </c>
+      <c r="C19" t="str">
+        <f>MasterData!AF19</f>
+        <v>No</v>
+      </c>
+      <c r="D19" t="str">
+        <f>MasterData!AG19</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="str">
+        <f>MasterData!AE20</f>
+        <v xml:space="preserve">No </v>
+      </c>
+      <c r="C20" t="str">
+        <f>MasterData!AF20</f>
+        <v>Yes</v>
+      </c>
+      <c r="D20" t="str">
+        <f>MasterData!AG20</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <f>MasterData!AE21</f>
+        <v>Yes</v>
+      </c>
+      <c r="C21" t="str">
+        <f>MasterData!AF21</f>
+        <v>Yes</v>
+      </c>
+      <c r="D21" t="str">
+        <f>MasterData!AG21</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
+        <f>MasterData!AE22</f>
+        <v xml:space="preserve">No </v>
+      </c>
+      <c r="C22" t="str">
+        <f>MasterData!AF22</f>
+        <v>No</v>
+      </c>
+      <c r="D22" t="str">
+        <f>MasterData!AG22</f>
         <v>Yes</v>
       </c>
     </row>
@@ -4331,14 +6695,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="B2:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
-      <selection activeCell="B12" sqref="B12:E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -4346,7 +6710,7 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>38</v>
       </c>
@@ -4360,7 +6724,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="str">
         <f>MasterData!AH3</f>
         <v>4111111111111111</v>
@@ -4378,7 +6742,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="str">
         <f>MasterData!AH4</f>
         <v>4111111111111111</v>
@@ -4396,7 +6760,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="str">
         <f>MasterData!AH5</f>
         <v>4111111111111111</v>
@@ -4414,7 +6778,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="str">
         <f>MasterData!AH6</f>
         <v>4111111111111111</v>
@@ -4432,7 +6796,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="str">
         <f>MasterData!AH7</f>
         <v>4111111111111111</v>
@@ -4450,7 +6814,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="str">
         <f>MasterData!AH8</f>
         <v>4111111111111111</v>
@@ -4468,7 +6832,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="str">
         <f>MasterData!AH9</f>
         <v>4111111111111111</v>
@@ -4486,7 +6850,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="str">
         <f>MasterData!AH10</f>
         <v>4111111111111111</v>
@@ -4504,7 +6868,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="str">
         <f>MasterData!AH11</f>
         <v>4111111111111111</v>
@@ -4522,7 +6886,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="str">
         <f>MasterData!AH12</f>
         <v>4111111111111111</v>
@@ -4540,7 +6904,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="str">
         <f>MasterData!AH13</f>
         <v>4111111111111111</v>
@@ -4555,6 +6919,168 @@
       </c>
       <c r="E13">
         <f>MasterData!AK13</f>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="str">
+        <f>MasterData!AH14</f>
+        <v>4111111111111111</v>
+      </c>
+      <c r="C14">
+        <f>MasterData!AI14</f>
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <f>MasterData!AJ14</f>
+        <v>2023</v>
+      </c>
+      <c r="E14">
+        <f>MasterData!AK14</f>
+        <v>542</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="str">
+        <f>MasterData!AH15</f>
+        <v>4111111111111111</v>
+      </c>
+      <c r="C15">
+        <f>MasterData!AI15</f>
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <f>MasterData!AJ15</f>
+        <v>2022</v>
+      </c>
+      <c r="E15">
+        <f>MasterData!AK15</f>
+        <v>629</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="str">
+        <f>MasterData!AH16</f>
+        <v>4111111111111111</v>
+      </c>
+      <c r="C16">
+        <f>MasterData!AI16</f>
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f>MasterData!AJ16</f>
+        <v>2020</v>
+      </c>
+      <c r="E16">
+        <f>MasterData!AK16</f>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="str">
+        <f>MasterData!AH17</f>
+        <v>4111111111111111</v>
+      </c>
+      <c r="C17">
+        <f>MasterData!AI17</f>
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <f>MasterData!AJ17</f>
+        <v>2023</v>
+      </c>
+      <c r="E17">
+        <f>MasterData!AK17</f>
+        <v>542</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="str">
+        <f>MasterData!AH18</f>
+        <v>4111111111111111</v>
+      </c>
+      <c r="C18">
+        <f>MasterData!AI18</f>
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <f>MasterData!AJ18</f>
+        <v>2022</v>
+      </c>
+      <c r="E18">
+        <f>MasterData!AK18</f>
+        <v>629</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="str">
+        <f>MasterData!AH19</f>
+        <v>4111111111111111</v>
+      </c>
+      <c r="C19">
+        <f>MasterData!AI19</f>
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f>MasterData!AJ19</f>
+        <v>2020</v>
+      </c>
+      <c r="E19">
+        <f>MasterData!AK19</f>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="str">
+        <f>MasterData!AH20</f>
+        <v>4111111111111111</v>
+      </c>
+      <c r="C20">
+        <f>MasterData!AI20</f>
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <f>MasterData!AJ20</f>
+        <v>2023</v>
+      </c>
+      <c r="E20">
+        <f>MasterData!AK20</f>
+        <v>542</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="str">
+        <f>MasterData!AH21</f>
+        <v>4111111111111111</v>
+      </c>
+      <c r="C21">
+        <f>MasterData!AI21</f>
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <f>MasterData!AJ21</f>
+        <v>2022</v>
+      </c>
+      <c r="E21">
+        <f>MasterData!AK21</f>
+        <v>629</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="str">
+        <f>MasterData!AH22</f>
+        <v>4111111111111111</v>
+      </c>
+      <c r="C22">
+        <f>MasterData!AI22</f>
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f>MasterData!AJ22</f>
+        <v>2020</v>
+      </c>
+      <c r="E22">
+        <f>MasterData!AK22</f>
         <v>289</v>
       </c>
     </row>

</xml_diff>